<commit_message>
NEW Project IP_calculation_Pro two files program 2.0 with def
</commit_message>
<xml_diff>
--- a/IP_calculation_Pro/Main_file_test.xlsx
+++ b/IP_calculation_Pro/Main_file_test.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1564,7 +1564,279 @@
         <v>256</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>45518.9317514573</v>
+        <v>45518.93175145833</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Медиамонитор</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ПРГС.465000.024</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>768</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1023</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>10.8.12.0</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>10.8.12.255</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>256</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>45518.93761497685</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Домик для Мышки Норушки</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>с трубой</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>769</v>
+      </c>
+      <c r="D35" t="n">
+        <v>776</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>10.6.23.0</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>10.6.23.7</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>8</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>45519.71073408565</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Коммутатор</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ПРГС.465000.028</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>969</v>
+      </c>
+      <c r="D36" t="n">
+        <v>974</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>10.8.15.0</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>10.8.15.5</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>6</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>45519.7180065162</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Домик для Мышки Норушки</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>без трубы</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>2560</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2569</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>10.6.20.1</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>10.6.20.10</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>10</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>45519.78871003472</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Домик для Мышки Норушки</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>без трубы</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>2570</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2580</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>10.6.20.11</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>10.6.20.21</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>11</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>45519.78922873842</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Домик для Мышки Норушки</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>без трубы</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>2581</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2880</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>10.6.20.22</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>10.6.21.65</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>300</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>45519.78981166667</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Домик для Мышки Норушки</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>без трубы</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>2881</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2885</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>10.6.21.66</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>10.6.21.70</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>5</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>45519.81906033565</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Домик для Мышки Норушки</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>без трубы</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>2886</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3145</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>10.6.21.71</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>10.6.22.74</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>260</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>45519.82235841767</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEW Project IP_calculation_Pro two files program 2.1 with def and checks
</commit_message>
<xml_diff>
--- a/IP_calculation_Pro/Main_file_test.xlsx
+++ b/IP_calculation_Pro/Main_file_test.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1718,7 +1718,7 @@
         <v>2570</v>
       </c>
       <c r="D38" t="n">
-        <v>2580</v>
+        <v>2826</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1727,14 +1727,14 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>10.6.20.21</t>
+          <t>10.6.21.11</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>11</v>
+        <v>257</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>45519.78922873842</v>
+        <v>45519.95326806713</v>
       </c>
     </row>
     <row r="39">
@@ -1749,26 +1749,26 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2581</v>
+        <v>2827</v>
       </c>
       <c r="D39" t="n">
-        <v>2880</v>
+        <v>3083</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>10.6.20.22</t>
+          <t>10.6.21.12</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>10.6.21.65</t>
+          <t>10.6.22.12</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>45519.78981166667</v>
+        <v>45519.95669515046</v>
       </c>
     </row>
     <row r="40">
@@ -1783,26 +1783,26 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2881</v>
+        <v>3084</v>
       </c>
       <c r="D40" t="n">
-        <v>2885</v>
+        <v>3340</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>10.6.21.66</t>
+          <t>10.6.22.13</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>10.6.21.70</t>
+          <t>10.6.23.13</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>5</v>
+        <v>257</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>45519.81906033565</v>
+        <v>45519.95785613426</v>
       </c>
     </row>
     <row r="41">
@@ -1817,26 +1817,60 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2886</v>
+        <v>3341</v>
       </c>
       <c r="D41" t="n">
-        <v>3145</v>
+        <v>3579</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>10.6.21.71</t>
+          <t>10.6.23.14</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>10.6.22.74</t>
+          <t>10.6.23.252</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>45519.82235841767</v>
+        <v>45519.96153725695</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Домик для Мышки Норушки</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>без трубы</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>3580</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3585</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>10.6.23.253</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>10.6.24.2</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>6</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>45519.96697361953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEW Project IP_calculation_Pro add order number and count check
</commit_message>
<xml_diff>
--- a/IP_calculation_Pro/Main_file_test.xlsx
+++ b/IP_calculation_Pro/Main_file_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\PycharmProjects\first_public_project\IP_calculation_Pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FEAD88-DF88-47F8-97BE-32BE308C9B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C707719B-43CB-4907-A061-5AFA47FB267D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="88">
   <si>
     <t>equipment_name</t>
   </si>
@@ -284,45 +284,6 @@
   </si>
   <si>
     <t>10.8.15.5</t>
-  </si>
-  <si>
-    <t>без трубы</t>
-  </si>
-  <si>
-    <t>10.6.20.1</t>
-  </si>
-  <si>
-    <t>10.6.20.10</t>
-  </si>
-  <si>
-    <t>10.6.20.11</t>
-  </si>
-  <si>
-    <t>10.6.21.11</t>
-  </si>
-  <si>
-    <t>10.6.21.12</t>
-  </si>
-  <si>
-    <t>10.6.22.12</t>
-  </si>
-  <si>
-    <t>10.6.22.13</t>
-  </si>
-  <si>
-    <t>10.6.23.13</t>
-  </si>
-  <si>
-    <t>10.6.23.14</t>
-  </si>
-  <si>
-    <t>10.6.23.252</t>
-  </si>
-  <si>
-    <t>10.6.23.253</t>
-  </si>
-  <si>
-    <t>10.6.24.3</t>
   </si>
 </sst>
 </file>
@@ -689,23 +650,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A39" sqref="A37:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1643,168 +1594,6 @@
         <v>45519.718006516203</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37">
-        <v>2560</v>
-      </c>
-      <c r="D37">
-        <v>2569</v>
-      </c>
-      <c r="E37" t="s">
-        <v>89</v>
-      </c>
-      <c r="F37" t="s">
-        <v>90</v>
-      </c>
-      <c r="G37">
-        <v>10</v>
-      </c>
-      <c r="H37" s="2">
-        <v>45519.788710034722</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38">
-        <v>2570</v>
-      </c>
-      <c r="D38">
-        <v>2826</v>
-      </c>
-      <c r="E38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38">
-        <v>257</v>
-      </c>
-      <c r="H38" s="2">
-        <v>45519.953268067133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39">
-        <v>2827</v>
-      </c>
-      <c r="D39">
-        <v>3083</v>
-      </c>
-      <c r="E39" t="s">
-        <v>93</v>
-      </c>
-      <c r="F39" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39">
-        <v>257</v>
-      </c>
-      <c r="H39" s="2">
-        <v>45519.95669515046</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40">
-        <v>3084</v>
-      </c>
-      <c r="D40">
-        <v>3340</v>
-      </c>
-      <c r="E40" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40">
-        <v>257</v>
-      </c>
-      <c r="H40" s="2">
-        <v>45519.957856134257</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41">
-        <v>3341</v>
-      </c>
-      <c r="D41">
-        <v>3579</v>
-      </c>
-      <c r="E41" t="s">
-        <v>97</v>
-      </c>
-      <c r="F41" t="s">
-        <v>98</v>
-      </c>
-      <c r="G41">
-        <v>239</v>
-      </c>
-      <c r="H41" s="2">
-        <v>45519.961537256953</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42">
-        <v>3580</v>
-      </c>
-      <c r="D42">
-        <v>3586</v>
-      </c>
-      <c r="E42" t="s">
-        <v>99</v>
-      </c>
-      <c r="F42" t="s">
-        <v>100</v>
-      </c>
-      <c r="G42">
-        <v>7</v>
-      </c>
-      <c r="H42" s="2">
-        <v>45520.377980613433</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H44" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>